<commit_message>
fix: antimony new parser
</commit_message>
<xml_diff>
--- a/LME/parser_beta_2.0/data/nbk_tenge.xlsx
+++ b/LME/parser_beta_2.0/data/nbk_tenge.xlsx
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1500"/>
+  <dimension ref="A1:D1502"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -21387,6 +21387,34 @@
         <v>494.63</v>
       </c>
     </row>
+    <row r="1501" spans="1:4">
+      <c r="A1501" s="1">
+        <v>1499</v>
+      </c>
+      <c r="B1501" s="2">
+        <v>46061</v>
+      </c>
+      <c r="C1501">
+        <v>1</v>
+      </c>
+      <c r="D1501">
+        <v>494.63</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:4">
+      <c r="A1502" s="1">
+        <v>1500</v>
+      </c>
+      <c r="B1502" s="2">
+        <v>46062</v>
+      </c>
+      <c r="C1502">
+        <v>1</v>
+      </c>
+      <c r="D1502">
+        <v>494.63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>